<commit_message>
add the ml lab
</commit_message>
<xml_diff>
--- a/program.xlsx
+++ b/program.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/teaching-bigdata/AA2425-unibo-mldm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC10480B991D78805BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2DD7AFD-1600-4452-87D2-EAE7C5DE7A9A}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10480B991D78805BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B0E8E08-B5A5-41CF-B229-0D8BB8A9A90A}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6660" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E17" sqref="A1:E17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +444,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -472,8 +472,8 @@
         <v>2</v>
       </c>
       <c r="E3" s="4">
-        <f>SUM($C$3:C3)/30</f>
-        <v>6.6666666666666666E-2</v>
+        <f>SUM($C$3:C3)/$C$1</f>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -488,8 +488,8 @@
         <v>2</v>
       </c>
       <c r="E4" s="4">
-        <f>SUM($C$3:C4)/30</f>
-        <v>0.13333333333333333</v>
+        <f>SUM($C$3:C4)/$C$1</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -504,8 +504,8 @@
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <f>SUM($C$3:C5)/30</f>
-        <v>0.2</v>
+        <f>SUM($C$3:C5)/$C$1</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -520,8 +520,8 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <f>SUM($C$3:C6)/30</f>
-        <v>0.26666666666666666</v>
+        <f>SUM($C$3:C6)/$C$1</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -536,8 +536,8 @@
         <v>2</v>
       </c>
       <c r="E7" s="4">
-        <f>SUM($C$3:C7)/30</f>
-        <v>0.33333333333333331</v>
+        <f>SUM($C$3:C7)/$C$1</f>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -552,8 +552,8 @@
         <v>2</v>
       </c>
       <c r="E8" s="4">
-        <f>SUM($C$3:C8)/30</f>
-        <v>0.4</v>
+        <f>SUM($C$3:C8)/$C$1</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -568,8 +568,8 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f>SUM($C$3:C9)/30</f>
-        <v>0.46666666666666667</v>
+        <f>SUM($C$3:C9)/$C$1</f>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -584,8 +584,8 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f>SUM($C$3:C10)/30</f>
-        <v>0.53333333333333333</v>
+        <f>SUM($C$3:C10)/$C$1</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -600,8 +600,8 @@
         <v>2</v>
       </c>
       <c r="E11" s="4">
-        <f>SUM($C$3:C11)/30</f>
-        <v>0.6</v>
+        <f>SUM($C$3:C11)/$C$1</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -616,8 +616,8 @@
         <v>2</v>
       </c>
       <c r="E12" s="4">
-        <f>SUM($C$3:C12)/30</f>
-        <v>0.66666666666666663</v>
+        <f>SUM($C$3:C12)/$C$1</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -632,8 +632,8 @@
         <v>2</v>
       </c>
       <c r="E13" s="4">
-        <f>SUM($C$3:C13)/30</f>
-        <v>0.73333333333333328</v>
+        <f>SUM($C$3:C13)/$C$1</f>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,12 +641,15 @@
         <f>A13+7</f>
         <v>45630</v>
       </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="4">
-        <f>SUM($C$3:C14)/30</f>
-        <v>0.8</v>
+        <f>SUM($C$3:C14)/$C$1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -654,12 +657,15 @@
         <f t="shared" si="0"/>
         <v>45637</v>
       </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="E15" s="4">
-        <f>SUM($C$3:C15)/30</f>
-        <v>0.8666666666666667</v>
+        <f>SUM($C$3:C15)/$C$1</f>
+        <v>1.0833333333333333</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -667,32 +673,17 @@
         <f t="shared" si="0"/>
         <v>45644</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="4">
-        <f>SUM($C$3:C16)/30</f>
-        <v>0.93333333333333335</v>
+        <f>SUM($C$3:C16)/$C$1</f>
+        <v>1.1666666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
-        <f t="shared" si="0"/>
-        <v>45651</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4">
-        <f>SUM($C$3:C17)/30</f>
-        <v>1</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="E17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>